<commit_message>
model version 8 training results
</commit_message>
<xml_diff>
--- a/work.xlsx
+++ b/work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ImanHeydardoost\dental_paper_1\Dental-XRay-YOLO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BFD995-6BDD-48ED-AC1E-F8E27A1AC9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310C4F94-ED5F-464D-B7A6-C58B7DD3818E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="109">
   <si>
     <t>number of models in series</t>
   </si>
@@ -352,21 +352,40 @@
     <t>inference time (ms)</t>
   </si>
   <si>
-    <t>mAP50 per Class</t>
-  </si>
-  <si>
-    <t>0.302
-0.864
-0.629
-0.922
-0.654
-0.954
-0.0939
-0.423
-0.302
-0.108
-0.174
-0.412</t>
+    <t>a_5_5</t>
+  </si>
+  <si>
+    <t>17/2/2026</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>18/2/2026</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>19/2/2026</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>20/2/2026</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>21/2/2026</t>
+  </si>
+  <si>
+    <t>xlarge</t>
   </si>
 </sst>
 </file>
@@ -374,7 +393,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -537,7 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,23 +612,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -619,6 +626,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -904,7 +920,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -987,12 +1003,24 @@
     </row>
     <row r="4" spans="1:7" ht="199.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
+        <v>13829</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="199.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -1102,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C9021C-4823-4BF4-BE12-B962A68061DC}">
   <dimension ref="A1:AX20"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1149,77 +1177,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19" t="s">
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19" t="s">
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19" t="s">
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19" t="s">
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="19"/>
-      <c r="AS1" s="19"/>
-      <c r="AT1" s="19" t="s">
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="AU1" s="19"/>
-      <c r="AV1" s="19" t="s">
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="AW1" s="19"/>
-      <c r="AX1" s="19"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
     </row>
     <row r="2" spans="1:50" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
+      <c r="A2" s="26"/>
       <c r="B2" s="12" t="s">
         <v>33</v>
       </c>
@@ -2345,24 +2373,23 @@
   <dimension ref="A1:S100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.69921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="6" width="16.796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.09765625" style="1" customWidth="1"/>
-    <col min="8" max="11" width="16.09765625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.19921875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.796875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.3984375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.69921875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="21.796875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="18.296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="1" customWidth="1"/>
+    <col min="6" max="7" width="16.796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.09765625" style="1" customWidth="1"/>
+    <col min="9" max="12" width="16.09765625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.19921875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.796875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.3984375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.69921875" style="1" customWidth="1"/>
     <col min="18" max="18" width="21.69921875" style="1" customWidth="1"/>
     <col min="19" max="19" width="14.09765625" style="1" customWidth="1"/>
     <col min="20" max="16384" width="8.8984375" style="1"/>
@@ -2372,58 +2399,58 @@
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="H1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="I1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="K1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="L1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="M1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="O1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="P1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="Q1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="R1" s="25" t="s">
+      <c r="R1" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="S1" s="21" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2434,169 +2461,362 @@
       <c r="B2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="D2" s="9">
+      <c r="E2" s="9">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="9">
+      <c r="I2" s="9">
         <v>0.01</v>
       </c>
-      <c r="I2" s="9">
+      <c r="J2" s="9">
         <v>16</v>
       </c>
-      <c r="J2" s="9">
+      <c r="K2" s="9">
         <v>100</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="22">
+      <c r="M2" s="19">
         <v>0.48627999999999999</v>
       </c>
-      <c r="M2" s="22">
+      <c r="N2" s="19">
         <v>0.26024999999999998</v>
       </c>
-      <c r="N2" s="22">
+      <c r="O2" s="19">
         <v>0.51575000000000004</v>
       </c>
-      <c r="O2" s="22">
+      <c r="P2" s="19">
         <v>0.52449999999999997</v>
       </c>
-      <c r="P2" s="22">
-        <f>2*(N2*O2)/(N2+O2)</f>
+      <c r="Q2" s="19">
+        <f>2*(O2*P2)/(O2+P2)</f>
         <v>0.52008819995193467</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="R2" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="S2" s="20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="R2" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="S2" s="23">
+      <c r="C3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J3" s="9">
+        <v>16</v>
+      </c>
+      <c r="K3" s="9">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="23"/>
+      <c r="L3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="M3" s="19">
+        <v>0.46614</v>
+      </c>
+      <c r="N3" s="19">
+        <v>0.23693</v>
+      </c>
+      <c r="O3" s="19">
+        <v>0.5343</v>
+      </c>
+      <c r="P3" s="19">
+        <v>0.44085999999999997</v>
+      </c>
+      <c r="Q3" s="19">
+        <f t="shared" ref="Q3:Q7" si="0">2*(O3*P3)/(O3+P3)</f>
+        <v>0.48310328151277737</v>
+      </c>
+      <c r="R3" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="S3" s="20">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="23"/>
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J4" s="9">
+        <v>16</v>
+      </c>
+      <c r="K4" s="9">
+        <v>100</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="19">
+        <v>0.53337000000000001</v>
+      </c>
+      <c r="N4" s="19">
+        <v>0.29136000000000001</v>
+      </c>
+      <c r="O4" s="19">
+        <v>0.57379999999999998</v>
+      </c>
+      <c r="P4" s="19">
+        <v>0.54252</v>
+      </c>
+      <c r="Q4" s="19">
+        <f t="shared" si="0"/>
+        <v>0.55772175720223593</v>
+      </c>
+      <c r="R4" s="19">
+        <v>1.7</v>
+      </c>
+      <c r="S4" s="20">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="23"/>
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J5" s="9">
+        <v>16</v>
+      </c>
+      <c r="K5" s="9">
+        <v>100</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="19">
+        <v>0.56028999999999995</v>
+      </c>
+      <c r="N5" s="19">
+        <v>0.31753999999999999</v>
+      </c>
+      <c r="O5" s="19">
+        <v>0.59638999999999998</v>
+      </c>
+      <c r="P5" s="19">
+        <v>0.55254999999999999</v>
+      </c>
+      <c r="Q5" s="19">
+        <f t="shared" si="0"/>
+        <v>0.57363360053614632</v>
+      </c>
+      <c r="R5" s="19">
+        <v>3.2</v>
+      </c>
+      <c r="S5" s="20">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="23"/>
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>1</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J6" s="9">
+        <v>16</v>
+      </c>
+      <c r="K6" s="9">
+        <v>100</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="19">
+        <v>0.57698000000000005</v>
+      </c>
+      <c r="N6" s="19">
+        <v>0.33145000000000002</v>
+      </c>
+      <c r="O6" s="19">
+        <v>0.628</v>
+      </c>
+      <c r="P6" s="19">
+        <v>0.57833000000000001</v>
+      </c>
+      <c r="Q6" s="19">
+        <f t="shared" si="0"/>
+        <v>0.60214243200450968</v>
+      </c>
+      <c r="R6" s="19">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="S6" s="20">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="23"/>
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J7" s="9">
+        <v>16</v>
+      </c>
+      <c r="K7" s="9">
+        <v>100</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="19">
+        <v>0.59257000000000004</v>
+      </c>
+      <c r="N7" s="19">
+        <v>0.35102</v>
+      </c>
+      <c r="O7" s="19">
+        <v>0.62219999999999998</v>
+      </c>
+      <c r="P7" s="19">
+        <v>0.58816000000000002</v>
+      </c>
+      <c r="Q7" s="19">
+        <f t="shared" si="0"/>
+        <v>0.6047013318351564</v>
+      </c>
+      <c r="R7" s="19"/>
+      <c r="S7" s="20">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -2604,20 +2824,20 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="23"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="20"/>
     </row>
     <row r="9" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -2625,20 +2845,20 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="23"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="20"/>
     </row>
     <row r="10" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -2646,20 +2866,20 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="23"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="20"/>
     </row>
     <row r="11" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -2667,20 +2887,20 @@
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="23"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="20"/>
     </row>
     <row r="12" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -2688,20 +2908,20 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="23"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="20"/>
     </row>
     <row r="13" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -2709,20 +2929,20 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="23"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="20"/>
     </row>
     <row r="14" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -2730,20 +2950,20 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="23"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="20"/>
     </row>
     <row r="15" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -2751,20 +2971,20 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="23"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="20"/>
     </row>
     <row r="16" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -2772,20 +2992,20 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-      <c r="S16" s="23"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="20"/>
     </row>
     <row r="17" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -2793,20 +3013,20 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="23"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="20"/>
     </row>
     <row r="18" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -2814,20 +3034,20 @@
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="23"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="20"/>
     </row>
     <row r="19" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -2835,20 +3055,20 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="23"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="20"/>
     </row>
     <row r="20" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -2856,20 +3076,20 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="23"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="20"/>
     </row>
     <row r="21" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
+      <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -2877,20 +3097,20 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="23"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="20"/>
     </row>
     <row r="22" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="8"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -2898,20 +3118,20 @@
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="23"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="20"/>
     </row>
     <row r="23" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -2919,20 +3139,20 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="23"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="20"/>
     </row>
     <row r="24" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
+      <c r="D24" s="8"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -2940,20 +3160,20 @@
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="23"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="20"/>
     </row>
     <row r="25" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
+      <c r="D25" s="8"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -2961,20 +3181,20 @@
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="23"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="20"/>
     </row>
     <row r="26" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
+      <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -2982,20 +3202,20 @@
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="23"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="20"/>
     </row>
     <row r="27" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
@@ -3003,20 +3223,20 @@
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="S27" s="23"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="20"/>
     </row>
     <row r="28" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
+      <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -3024,20 +3244,20 @@
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="23"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="20"/>
     </row>
     <row r="29" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
+      <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -3045,20 +3265,20 @@
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-      <c r="Q29" s="22"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="23"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="20"/>
     </row>
     <row r="30" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
+      <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -3066,20 +3286,20 @@
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="22"/>
-      <c r="S30" s="23"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="20"/>
     </row>
     <row r="31" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
+      <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -3087,20 +3307,20 @@
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="22"/>
-      <c r="S31" s="23"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="20"/>
     </row>
     <row r="32" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
+      <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -3108,20 +3328,20 @@
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="22"/>
-      <c r="S32" s="23"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="20"/>
     </row>
     <row r="33" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
+      <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -3129,20 +3349,20 @@
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="22"/>
-      <c r="S33" s="23"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="20"/>
     </row>
     <row r="34" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
+      <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -3150,20 +3370,20 @@
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="23"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="20"/>
     </row>
     <row r="35" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
+      <c r="D35" s="8"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -3171,20 +3391,20 @@
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="23"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="20"/>
     </row>
     <row r="36" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
+      <c r="D36" s="8"/>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -3192,20 +3412,20 @@
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="22"/>
-      <c r="S36" s="23"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="20"/>
     </row>
     <row r="37" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
+      <c r="D37" s="8"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -3213,20 +3433,20 @@
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="23"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="20"/>
     </row>
     <row r="38" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
+      <c r="D38" s="8"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
@@ -3234,20 +3454,20 @@
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="23"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="20"/>
     </row>
     <row r="39" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
+      <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
@@ -3255,20 +3475,20 @@
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="22"/>
-      <c r="P39" s="22"/>
-      <c r="Q39" s="22"/>
-      <c r="R39" s="22"/>
-      <c r="S39" s="23"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="20"/>
     </row>
     <row r="40" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
+      <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
@@ -3276,20 +3496,20 @@
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="22"/>
-      <c r="S40" s="23"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="20"/>
     </row>
     <row r="41" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
+      <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -3297,20 +3517,20 @@
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="22"/>
-      <c r="Q41" s="22"/>
-      <c r="R41" s="22"/>
-      <c r="S41" s="23"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="20"/>
     </row>
     <row r="42" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
+      <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -3318,20 +3538,20 @@
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="22"/>
-      <c r="S42" s="23"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="20"/>
     </row>
     <row r="43" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
+      <c r="D43" s="8"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
@@ -3339,20 +3559,20 @@
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
-      <c r="P43" s="22"/>
-      <c r="Q43" s="22"/>
-      <c r="R43" s="22"/>
-      <c r="S43" s="23"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="20"/>
     </row>
     <row r="44" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
+      <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -3360,20 +3580,20 @@
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="23"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="20"/>
     </row>
     <row r="45" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
+      <c r="D45" s="8"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
@@ -3381,20 +3601,20 @@
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
-      <c r="R45" s="22"/>
-      <c r="S45" s="23"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="20"/>
     </row>
     <row r="46" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
+      <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
@@ -3402,20 +3622,20 @@
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22"/>
-      <c r="R46" s="22"/>
-      <c r="S46" s="23"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="20"/>
     </row>
     <row r="47" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
+      <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
@@ -3423,20 +3643,20 @@
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="22"/>
-      <c r="Q47" s="22"/>
-      <c r="R47" s="22"/>
-      <c r="S47" s="23"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="20"/>
     </row>
     <row r="48" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
+      <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
@@ -3444,20 +3664,20 @@
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
-      <c r="R48" s="22"/>
-      <c r="S48" s="23"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="20"/>
     </row>
     <row r="49" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
+      <c r="D49" s="8"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
@@ -3465,20 +3685,20 @@
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="22"/>
-      <c r="O49" s="22"/>
-      <c r="P49" s="22"/>
-      <c r="Q49" s="22"/>
-      <c r="R49" s="22"/>
-      <c r="S49" s="23"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="O49" s="19"/>
+      <c r="P49" s="19"/>
+      <c r="Q49" s="19"/>
+      <c r="R49" s="19"/>
+      <c r="S49" s="20"/>
     </row>
     <row r="50" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
+      <c r="D50" s="8"/>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
@@ -3486,20 +3706,20 @@
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="22"/>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="22"/>
-      <c r="S50" s="23"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="20"/>
     </row>
     <row r="51" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
+      <c r="D51" s="8"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
@@ -3507,20 +3727,20 @@
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
-      <c r="O51" s="22"/>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="23"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="19"/>
+      <c r="S51" s="20"/>
     </row>
     <row r="52" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
+      <c r="D52" s="8"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
@@ -3528,20 +3748,20 @@
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
-      <c r="L52" s="22"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="22"/>
-      <c r="O52" s="22"/>
-      <c r="P52" s="22"/>
-      <c r="Q52" s="22"/>
-      <c r="R52" s="22"/>
-      <c r="S52" s="23"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="19"/>
+      <c r="S52" s="20"/>
     </row>
     <row r="53" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
+      <c r="D53" s="8"/>
       <c r="E53" s="9"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
@@ -3549,20 +3769,20 @@
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
-      <c r="L53" s="22"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="22"/>
-      <c r="O53" s="22"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="22"/>
-      <c r="S53" s="23"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="19"/>
+      <c r="P53" s="19"/>
+      <c r="Q53" s="19"/>
+      <c r="R53" s="19"/>
+      <c r="S53" s="20"/>
     </row>
     <row r="54" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
+      <c r="D54" s="8"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
@@ -3570,20 +3790,20 @@
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
-      <c r="L54" s="22"/>
-      <c r="M54" s="22"/>
-      <c r="N54" s="22"/>
-      <c r="O54" s="22"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="22"/>
-      <c r="S54" s="23"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="19"/>
+      <c r="O54" s="19"/>
+      <c r="P54" s="19"/>
+      <c r="Q54" s="19"/>
+      <c r="R54" s="19"/>
+      <c r="S54" s="20"/>
     </row>
     <row r="55" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
+      <c r="D55" s="8"/>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
@@ -3591,20 +3811,20 @@
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
-      <c r="L55" s="22"/>
-      <c r="M55" s="22"/>
-      <c r="N55" s="22"/>
-      <c r="O55" s="22"/>
-      <c r="P55" s="22"/>
-      <c r="Q55" s="22"/>
-      <c r="R55" s="22"/>
-      <c r="S55" s="23"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="19"/>
+      <c r="O55" s="19"/>
+      <c r="P55" s="19"/>
+      <c r="Q55" s="19"/>
+      <c r="R55" s="19"/>
+      <c r="S55" s="20"/>
     </row>
     <row r="56" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
+      <c r="D56" s="8"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
@@ -3612,20 +3832,20 @@
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
-      <c r="L56" s="22"/>
-      <c r="M56" s="22"/>
-      <c r="N56" s="22"/>
-      <c r="O56" s="22"/>
-      <c r="P56" s="22"/>
-      <c r="Q56" s="22"/>
-      <c r="R56" s="22"/>
-      <c r="S56" s="23"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="19"/>
+      <c r="N56" s="19"/>
+      <c r="O56" s="19"/>
+      <c r="P56" s="19"/>
+      <c r="Q56" s="19"/>
+      <c r="R56" s="19"/>
+      <c r="S56" s="20"/>
     </row>
     <row r="57" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
+      <c r="D57" s="8"/>
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
@@ -3633,20 +3853,20 @@
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
-      <c r="L57" s="22"/>
-      <c r="M57" s="22"/>
-      <c r="N57" s="22"/>
-      <c r="O57" s="22"/>
-      <c r="P57" s="22"/>
-      <c r="Q57" s="22"/>
-      <c r="R57" s="22"/>
-      <c r="S57" s="23"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="19"/>
+      <c r="O57" s="19"/>
+      <c r="P57" s="19"/>
+      <c r="Q57" s="19"/>
+      <c r="R57" s="19"/>
+      <c r="S57" s="20"/>
     </row>
     <row r="58" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
+      <c r="D58" s="8"/>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -3654,20 +3874,20 @@
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="22"/>
-      <c r="N58" s="22"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
-      <c r="R58" s="22"/>
-      <c r="S58" s="23"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="19"/>
+      <c r="N58" s="19"/>
+      <c r="O58" s="19"/>
+      <c r="P58" s="19"/>
+      <c r="Q58" s="19"/>
+      <c r="R58" s="19"/>
+      <c r="S58" s="20"/>
     </row>
     <row r="59" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
-      <c r="D59" s="9"/>
+      <c r="D59" s="8"/>
       <c r="E59" s="9"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -3675,20 +3895,20 @@
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="22"/>
-      <c r="N59" s="22"/>
-      <c r="O59" s="22"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="22"/>
-      <c r="R59" s="22"/>
-      <c r="S59" s="23"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19"/>
+      <c r="O59" s="19"/>
+      <c r="P59" s="19"/>
+      <c r="Q59" s="19"/>
+      <c r="R59" s="19"/>
+      <c r="S59" s="20"/>
     </row>
     <row r="60" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
-      <c r="D60" s="9"/>
+      <c r="D60" s="8"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
@@ -3696,20 +3916,20 @@
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="22"/>
-      <c r="N60" s="22"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="22"/>
-      <c r="Q60" s="22"/>
-      <c r="R60" s="22"/>
-      <c r="S60" s="23"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="19"/>
+      <c r="N60" s="19"/>
+      <c r="O60" s="19"/>
+      <c r="P60" s="19"/>
+      <c r="Q60" s="19"/>
+      <c r="R60" s="19"/>
+      <c r="S60" s="20"/>
     </row>
     <row r="61" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
+      <c r="D61" s="8"/>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
@@ -3717,20 +3937,20 @@
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="22"/>
-      <c r="N61" s="22"/>
-      <c r="O61" s="22"/>
-      <c r="P61" s="22"/>
-      <c r="Q61" s="22"/>
-      <c r="R61" s="22"/>
-      <c r="S61" s="23"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="19"/>
+      <c r="N61" s="19"/>
+      <c r="O61" s="19"/>
+      <c r="P61" s="19"/>
+      <c r="Q61" s="19"/>
+      <c r="R61" s="19"/>
+      <c r="S61" s="20"/>
     </row>
     <row r="62" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
+      <c r="D62" s="8"/>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
@@ -3738,20 +3958,20 @@
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
-      <c r="L62" s="22"/>
-      <c r="M62" s="22"/>
-      <c r="N62" s="22"/>
-      <c r="O62" s="22"/>
-      <c r="P62" s="22"/>
-      <c r="Q62" s="22"/>
-      <c r="R62" s="22"/>
-      <c r="S62" s="23"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="19"/>
+      <c r="N62" s="19"/>
+      <c r="O62" s="19"/>
+      <c r="P62" s="19"/>
+      <c r="Q62" s="19"/>
+      <c r="R62" s="19"/>
+      <c r="S62" s="20"/>
     </row>
     <row r="63" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
-      <c r="D63" s="9"/>
+      <c r="D63" s="8"/>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
@@ -3759,20 +3979,20 @@
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="22"/>
-      <c r="N63" s="22"/>
-      <c r="O63" s="22"/>
-      <c r="P63" s="22"/>
-      <c r="Q63" s="22"/>
-      <c r="R63" s="22"/>
-      <c r="S63" s="23"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="19"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="19"/>
+      <c r="P63" s="19"/>
+      <c r="Q63" s="19"/>
+      <c r="R63" s="19"/>
+      <c r="S63" s="20"/>
     </row>
     <row r="64" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
-      <c r="D64" s="9"/>
+      <c r="D64" s="8"/>
       <c r="E64" s="9"/>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
@@ -3780,20 +4000,20 @@
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="22"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="22"/>
-      <c r="R64" s="22"/>
-      <c r="S64" s="23"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="19"/>
+      <c r="N64" s="19"/>
+      <c r="O64" s="19"/>
+      <c r="P64" s="19"/>
+      <c r="Q64" s="19"/>
+      <c r="R64" s="19"/>
+      <c r="S64" s="20"/>
     </row>
     <row r="65" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="9"/>
+      <c r="D65" s="8"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
@@ -3801,20 +4021,20 @@
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
-      <c r="L65" s="22"/>
-      <c r="M65" s="22"/>
-      <c r="N65" s="22"/>
-      <c r="O65" s="22"/>
-      <c r="P65" s="22"/>
-      <c r="Q65" s="22"/>
-      <c r="R65" s="22"/>
-      <c r="S65" s="23"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="19"/>
+      <c r="N65" s="19"/>
+      <c r="O65" s="19"/>
+      <c r="P65" s="19"/>
+      <c r="Q65" s="19"/>
+      <c r="R65" s="19"/>
+      <c r="S65" s="20"/>
     </row>
     <row r="66" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
-      <c r="D66" s="9"/>
+      <c r="D66" s="8"/>
       <c r="E66" s="9"/>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
@@ -3822,20 +4042,20 @@
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
-      <c r="L66" s="22"/>
-      <c r="M66" s="22"/>
-      <c r="N66" s="22"/>
-      <c r="O66" s="22"/>
-      <c r="P66" s="22"/>
-      <c r="Q66" s="22"/>
-      <c r="R66" s="22"/>
-      <c r="S66" s="23"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="19"/>
+      <c r="N66" s="19"/>
+      <c r="O66" s="19"/>
+      <c r="P66" s="19"/>
+      <c r="Q66" s="19"/>
+      <c r="R66" s="19"/>
+      <c r="S66" s="20"/>
     </row>
     <row r="67" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="9"/>
+      <c r="D67" s="8"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
@@ -3843,20 +4063,20 @@
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
-      <c r="L67" s="22"/>
-      <c r="M67" s="22"/>
-      <c r="N67" s="22"/>
-      <c r="O67" s="22"/>
-      <c r="P67" s="22"/>
-      <c r="Q67" s="22"/>
-      <c r="R67" s="22"/>
-      <c r="S67" s="23"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="19"/>
+      <c r="N67" s="19"/>
+      <c r="O67" s="19"/>
+      <c r="P67" s="19"/>
+      <c r="Q67" s="19"/>
+      <c r="R67" s="19"/>
+      <c r="S67" s="20"/>
     </row>
     <row r="68" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="9"/>
+      <c r="D68" s="8"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
@@ -3864,20 +4084,20 @@
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
-      <c r="L68" s="22"/>
-      <c r="M68" s="22"/>
-      <c r="N68" s="22"/>
-      <c r="O68" s="22"/>
-      <c r="P68" s="22"/>
-      <c r="Q68" s="22"/>
-      <c r="R68" s="22"/>
-      <c r="S68" s="23"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="19"/>
+      <c r="N68" s="19"/>
+      <c r="O68" s="19"/>
+      <c r="P68" s="19"/>
+      <c r="Q68" s="19"/>
+      <c r="R68" s="19"/>
+      <c r="S68" s="20"/>
     </row>
     <row r="69" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
-      <c r="D69" s="9"/>
+      <c r="D69" s="8"/>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
@@ -3885,20 +4105,20 @@
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
-      <c r="L69" s="22"/>
-      <c r="M69" s="22"/>
-      <c r="N69" s="22"/>
-      <c r="O69" s="22"/>
-      <c r="P69" s="22"/>
-      <c r="Q69" s="22"/>
-      <c r="R69" s="22"/>
-      <c r="S69" s="23"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="19"/>
+      <c r="N69" s="19"/>
+      <c r="O69" s="19"/>
+      <c r="P69" s="19"/>
+      <c r="Q69" s="19"/>
+      <c r="R69" s="19"/>
+      <c r="S69" s="20"/>
     </row>
     <row r="70" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="9"/>
+      <c r="D70" s="8"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
@@ -3906,20 +4126,20 @@
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
-      <c r="L70" s="22"/>
-      <c r="M70" s="22"/>
-      <c r="N70" s="22"/>
-      <c r="O70" s="22"/>
-      <c r="P70" s="22"/>
-      <c r="Q70" s="22"/>
-      <c r="R70" s="22"/>
-      <c r="S70" s="23"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="19"/>
+      <c r="N70" s="19"/>
+      <c r="O70" s="19"/>
+      <c r="P70" s="19"/>
+      <c r="Q70" s="19"/>
+      <c r="R70" s="19"/>
+      <c r="S70" s="20"/>
     </row>
     <row r="71" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="9"/>
+      <c r="D71" s="8"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
@@ -3927,20 +4147,20 @@
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
-      <c r="L71" s="22"/>
-      <c r="M71" s="22"/>
-      <c r="N71" s="22"/>
-      <c r="O71" s="22"/>
-      <c r="P71" s="22"/>
-      <c r="Q71" s="22"/>
-      <c r="R71" s="22"/>
-      <c r="S71" s="23"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="19"/>
+      <c r="N71" s="19"/>
+      <c r="O71" s="19"/>
+      <c r="P71" s="19"/>
+      <c r="Q71" s="19"/>
+      <c r="R71" s="19"/>
+      <c r="S71" s="20"/>
     </row>
     <row r="72" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="9"/>
+      <c r="D72" s="8"/>
       <c r="E72" s="9"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
@@ -3948,20 +4168,20 @@
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
-      <c r="L72" s="22"/>
-      <c r="M72" s="22"/>
-      <c r="N72" s="22"/>
-      <c r="O72" s="22"/>
-      <c r="P72" s="22"/>
-      <c r="Q72" s="22"/>
-      <c r="R72" s="22"/>
-      <c r="S72" s="23"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="19"/>
+      <c r="N72" s="19"/>
+      <c r="O72" s="19"/>
+      <c r="P72" s="19"/>
+      <c r="Q72" s="19"/>
+      <c r="R72" s="19"/>
+      <c r="S72" s="20"/>
     </row>
     <row r="73" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="9"/>
+      <c r="D73" s="8"/>
       <c r="E73" s="9"/>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
@@ -3969,20 +4189,20 @@
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
-      <c r="L73" s="22"/>
-      <c r="M73" s="22"/>
-      <c r="N73" s="22"/>
-      <c r="O73" s="22"/>
-      <c r="P73" s="22"/>
-      <c r="Q73" s="22"/>
-      <c r="R73" s="22"/>
-      <c r="S73" s="23"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="19"/>
+      <c r="N73" s="19"/>
+      <c r="O73" s="19"/>
+      <c r="P73" s="19"/>
+      <c r="Q73" s="19"/>
+      <c r="R73" s="19"/>
+      <c r="S73" s="20"/>
     </row>
     <row r="74" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="9"/>
+      <c r="D74" s="8"/>
       <c r="E74" s="9"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
@@ -3990,20 +4210,20 @@
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
-      <c r="L74" s="22"/>
-      <c r="M74" s="22"/>
-      <c r="N74" s="22"/>
-      <c r="O74" s="22"/>
-      <c r="P74" s="22"/>
-      <c r="Q74" s="22"/>
-      <c r="R74" s="22"/>
-      <c r="S74" s="23"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="19"/>
+      <c r="N74" s="19"/>
+      <c r="O74" s="19"/>
+      <c r="P74" s="19"/>
+      <c r="Q74" s="19"/>
+      <c r="R74" s="19"/>
+      <c r="S74" s="20"/>
     </row>
     <row r="75" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="9"/>
+      <c r="D75" s="8"/>
       <c r="E75" s="9"/>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
@@ -4011,20 +4231,20 @@
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
-      <c r="L75" s="22"/>
-      <c r="M75" s="22"/>
-      <c r="N75" s="22"/>
-      <c r="O75" s="22"/>
-      <c r="P75" s="22"/>
-      <c r="Q75" s="22"/>
-      <c r="R75" s="22"/>
-      <c r="S75" s="23"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="19"/>
+      <c r="N75" s="19"/>
+      <c r="O75" s="19"/>
+      <c r="P75" s="19"/>
+      <c r="Q75" s="19"/>
+      <c r="R75" s="19"/>
+      <c r="S75" s="20"/>
     </row>
     <row r="76" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="9"/>
+      <c r="D76" s="8"/>
       <c r="E76" s="9"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
@@ -4032,20 +4252,20 @@
       <c r="I76" s="9"/>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
-      <c r="L76" s="22"/>
-      <c r="M76" s="22"/>
-      <c r="N76" s="22"/>
-      <c r="O76" s="22"/>
-      <c r="P76" s="22"/>
-      <c r="Q76" s="22"/>
-      <c r="R76" s="22"/>
-      <c r="S76" s="23"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="19"/>
+      <c r="N76" s="19"/>
+      <c r="O76" s="19"/>
+      <c r="P76" s="19"/>
+      <c r="Q76" s="19"/>
+      <c r="R76" s="19"/>
+      <c r="S76" s="20"/>
     </row>
     <row r="77" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="9"/>
+      <c r="D77" s="8"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
@@ -4053,20 +4273,20 @@
       <c r="I77" s="9"/>
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
-      <c r="L77" s="22"/>
-      <c r="M77" s="22"/>
-      <c r="N77" s="22"/>
-      <c r="O77" s="22"/>
-      <c r="P77" s="22"/>
-      <c r="Q77" s="22"/>
-      <c r="R77" s="22"/>
-      <c r="S77" s="23"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="19"/>
+      <c r="N77" s="19"/>
+      <c r="O77" s="19"/>
+      <c r="P77" s="19"/>
+      <c r="Q77" s="19"/>
+      <c r="R77" s="19"/>
+      <c r="S77" s="20"/>
     </row>
     <row r="78" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="9"/>
+      <c r="D78" s="8"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
@@ -4074,20 +4294,20 @@
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
-      <c r="L78" s="22"/>
-      <c r="M78" s="22"/>
-      <c r="N78" s="22"/>
-      <c r="O78" s="22"/>
-      <c r="P78" s="22"/>
-      <c r="Q78" s="22"/>
-      <c r="R78" s="22"/>
-      <c r="S78" s="23"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="19"/>
+      <c r="N78" s="19"/>
+      <c r="O78" s="19"/>
+      <c r="P78" s="19"/>
+      <c r="Q78" s="19"/>
+      <c r="R78" s="19"/>
+      <c r="S78" s="20"/>
     </row>
     <row r="79" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="9"/>
+      <c r="D79" s="8"/>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
@@ -4095,20 +4315,20 @@
       <c r="I79" s="9"/>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
-      <c r="L79" s="22"/>
-      <c r="M79" s="22"/>
-      <c r="N79" s="22"/>
-      <c r="O79" s="22"/>
-      <c r="P79" s="22"/>
-      <c r="Q79" s="22"/>
-      <c r="R79" s="22"/>
-      <c r="S79" s="23"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="19"/>
+      <c r="N79" s="19"/>
+      <c r="O79" s="19"/>
+      <c r="P79" s="19"/>
+      <c r="Q79" s="19"/>
+      <c r="R79" s="19"/>
+      <c r="S79" s="20"/>
     </row>
     <row r="80" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="9"/>
+      <c r="D80" s="8"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
@@ -4116,20 +4336,20 @@
       <c r="I80" s="9"/>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
-      <c r="L80" s="22"/>
-      <c r="M80" s="22"/>
-      <c r="N80" s="22"/>
-      <c r="O80" s="22"/>
-      <c r="P80" s="22"/>
-      <c r="Q80" s="22"/>
-      <c r="R80" s="22"/>
-      <c r="S80" s="23"/>
+      <c r="L80" s="9"/>
+      <c r="M80" s="19"/>
+      <c r="N80" s="19"/>
+      <c r="O80" s="19"/>
+      <c r="P80" s="19"/>
+      <c r="Q80" s="19"/>
+      <c r="R80" s="19"/>
+      <c r="S80" s="20"/>
     </row>
     <row r="81" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
-      <c r="D81" s="9"/>
+      <c r="D81" s="8"/>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
@@ -4137,20 +4357,20 @@
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
-      <c r="L81" s="22"/>
-      <c r="M81" s="22"/>
-      <c r="N81" s="22"/>
-      <c r="O81" s="22"/>
-      <c r="P81" s="22"/>
-      <c r="Q81" s="22"/>
-      <c r="R81" s="22"/>
-      <c r="S81" s="23"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="19"/>
+      <c r="N81" s="19"/>
+      <c r="O81" s="19"/>
+      <c r="P81" s="19"/>
+      <c r="Q81" s="19"/>
+      <c r="R81" s="19"/>
+      <c r="S81" s="20"/>
     </row>
     <row r="82" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
-      <c r="D82" s="9"/>
+      <c r="D82" s="8"/>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
@@ -4158,20 +4378,20 @@
       <c r="I82" s="9"/>
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
-      <c r="L82" s="22"/>
-      <c r="M82" s="22"/>
-      <c r="N82" s="22"/>
-      <c r="O82" s="22"/>
-      <c r="P82" s="22"/>
-      <c r="Q82" s="22"/>
-      <c r="R82" s="22"/>
-      <c r="S82" s="23"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="19"/>
+      <c r="N82" s="19"/>
+      <c r="O82" s="19"/>
+      <c r="P82" s="19"/>
+      <c r="Q82" s="19"/>
+      <c r="R82" s="19"/>
+      <c r="S82" s="20"/>
     </row>
     <row r="83" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="9"/>
+      <c r="D83" s="8"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
@@ -4179,20 +4399,20 @@
       <c r="I83" s="9"/>
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
-      <c r="L83" s="22"/>
-      <c r="M83" s="22"/>
-      <c r="N83" s="22"/>
-      <c r="O83" s="22"/>
-      <c r="P83" s="22"/>
-      <c r="Q83" s="22"/>
-      <c r="R83" s="22"/>
-      <c r="S83" s="23"/>
+      <c r="L83" s="9"/>
+      <c r="M83" s="19"/>
+      <c r="N83" s="19"/>
+      <c r="O83" s="19"/>
+      <c r="P83" s="19"/>
+      <c r="Q83" s="19"/>
+      <c r="R83" s="19"/>
+      <c r="S83" s="20"/>
     </row>
     <row r="84" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
-      <c r="D84" s="9"/>
+      <c r="D84" s="8"/>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
@@ -4200,20 +4420,20 @@
       <c r="I84" s="9"/>
       <c r="J84" s="9"/>
       <c r="K84" s="9"/>
-      <c r="L84" s="22"/>
-      <c r="M84" s="22"/>
-      <c r="N84" s="22"/>
-      <c r="O84" s="22"/>
-      <c r="P84" s="22"/>
-      <c r="Q84" s="22"/>
-      <c r="R84" s="22"/>
-      <c r="S84" s="23"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="19"/>
+      <c r="N84" s="19"/>
+      <c r="O84" s="19"/>
+      <c r="P84" s="19"/>
+      <c r="Q84" s="19"/>
+      <c r="R84" s="19"/>
+      <c r="S84" s="20"/>
     </row>
     <row r="85" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
-      <c r="D85" s="9"/>
+      <c r="D85" s="8"/>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
@@ -4221,20 +4441,20 @@
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
       <c r="K85" s="9"/>
-      <c r="L85" s="22"/>
-      <c r="M85" s="22"/>
-      <c r="N85" s="22"/>
-      <c r="O85" s="22"/>
-      <c r="P85" s="22"/>
-      <c r="Q85" s="22"/>
-      <c r="R85" s="22"/>
-      <c r="S85" s="23"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="19"/>
+      <c r="N85" s="19"/>
+      <c r="O85" s="19"/>
+      <c r="P85" s="19"/>
+      <c r="Q85" s="19"/>
+      <c r="R85" s="19"/>
+      <c r="S85" s="20"/>
     </row>
     <row r="86" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
-      <c r="D86" s="9"/>
+      <c r="D86" s="8"/>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
@@ -4242,20 +4462,20 @@
       <c r="I86" s="9"/>
       <c r="J86" s="9"/>
       <c r="K86" s="9"/>
-      <c r="L86" s="22"/>
-      <c r="M86" s="22"/>
-      <c r="N86" s="22"/>
-      <c r="O86" s="22"/>
-      <c r="P86" s="22"/>
-      <c r="Q86" s="22"/>
-      <c r="R86" s="22"/>
-      <c r="S86" s="23"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="19"/>
+      <c r="N86" s="19"/>
+      <c r="O86" s="19"/>
+      <c r="P86" s="19"/>
+      <c r="Q86" s="19"/>
+      <c r="R86" s="19"/>
+      <c r="S86" s="20"/>
     </row>
     <row r="87" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
-      <c r="D87" s="9"/>
+      <c r="D87" s="8"/>
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
       <c r="G87" s="9"/>
@@ -4263,20 +4483,20 @@
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
       <c r="K87" s="9"/>
-      <c r="L87" s="22"/>
-      <c r="M87" s="22"/>
-      <c r="N87" s="22"/>
-      <c r="O87" s="22"/>
-      <c r="P87" s="22"/>
-      <c r="Q87" s="22"/>
-      <c r="R87" s="22"/>
-      <c r="S87" s="23"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="19"/>
+      <c r="N87" s="19"/>
+      <c r="O87" s="19"/>
+      <c r="P87" s="19"/>
+      <c r="Q87" s="19"/>
+      <c r="R87" s="19"/>
+      <c r="S87" s="20"/>
     </row>
     <row r="88" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="9"/>
+      <c r="D88" s="8"/>
       <c r="E88" s="9"/>
       <c r="F88" s="9"/>
       <c r="G88" s="9"/>
@@ -4284,20 +4504,20 @@
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
-      <c r="L88" s="22"/>
-      <c r="M88" s="22"/>
-      <c r="N88" s="22"/>
-      <c r="O88" s="22"/>
-      <c r="P88" s="22"/>
-      <c r="Q88" s="22"/>
-      <c r="R88" s="22"/>
-      <c r="S88" s="23"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="19"/>
+      <c r="N88" s="19"/>
+      <c r="O88" s="19"/>
+      <c r="P88" s="19"/>
+      <c r="Q88" s="19"/>
+      <c r="R88" s="19"/>
+      <c r="S88" s="20"/>
     </row>
     <row r="89" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
-      <c r="D89" s="9"/>
+      <c r="D89" s="8"/>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
       <c r="G89" s="9"/>
@@ -4305,20 +4525,20 @@
       <c r="I89" s="9"/>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
-      <c r="L89" s="22"/>
-      <c r="M89" s="22"/>
-      <c r="N89" s="22"/>
-      <c r="O89" s="22"/>
-      <c r="P89" s="22"/>
-      <c r="Q89" s="22"/>
-      <c r="R89" s="22"/>
-      <c r="S89" s="23"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="19"/>
+      <c r="N89" s="19"/>
+      <c r="O89" s="19"/>
+      <c r="P89" s="19"/>
+      <c r="Q89" s="19"/>
+      <c r="R89" s="19"/>
+      <c r="S89" s="20"/>
     </row>
     <row r="90" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
-      <c r="D90" s="9"/>
+      <c r="D90" s="8"/>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
@@ -4326,20 +4546,20 @@
       <c r="I90" s="9"/>
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
-      <c r="L90" s="22"/>
-      <c r="M90" s="22"/>
-      <c r="N90" s="22"/>
-      <c r="O90" s="22"/>
-      <c r="P90" s="22"/>
-      <c r="Q90" s="22"/>
-      <c r="R90" s="22"/>
-      <c r="S90" s="23"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="19"/>
+      <c r="N90" s="19"/>
+      <c r="O90" s="19"/>
+      <c r="P90" s="19"/>
+      <c r="Q90" s="19"/>
+      <c r="R90" s="19"/>
+      <c r="S90" s="20"/>
     </row>
     <row r="91" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
-      <c r="D91" s="9"/>
+      <c r="D91" s="8"/>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
       <c r="G91" s="9"/>
@@ -4347,20 +4567,20 @@
       <c r="I91" s="9"/>
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
-      <c r="L91" s="22"/>
-      <c r="M91" s="22"/>
-      <c r="N91" s="22"/>
-      <c r="O91" s="22"/>
-      <c r="P91" s="22"/>
-      <c r="Q91" s="22"/>
-      <c r="R91" s="22"/>
-      <c r="S91" s="23"/>
+      <c r="L91" s="9"/>
+      <c r="M91" s="19"/>
+      <c r="N91" s="19"/>
+      <c r="O91" s="19"/>
+      <c r="P91" s="19"/>
+      <c r="Q91" s="19"/>
+      <c r="R91" s="19"/>
+      <c r="S91" s="20"/>
     </row>
     <row r="92" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
-      <c r="D92" s="9"/>
+      <c r="D92" s="8"/>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
       <c r="G92" s="9"/>
@@ -4368,20 +4588,20 @@
       <c r="I92" s="9"/>
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
-      <c r="L92" s="22"/>
-      <c r="M92" s="22"/>
-      <c r="N92" s="22"/>
-      <c r="O92" s="22"/>
-      <c r="P92" s="22"/>
-      <c r="Q92" s="22"/>
-      <c r="R92" s="22"/>
-      <c r="S92" s="23"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="19"/>
+      <c r="N92" s="19"/>
+      <c r="O92" s="19"/>
+      <c r="P92" s="19"/>
+      <c r="Q92" s="19"/>
+      <c r="R92" s="19"/>
+      <c r="S92" s="20"/>
     </row>
     <row r="93" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
-      <c r="D93" s="9"/>
+      <c r="D93" s="8"/>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
       <c r="G93" s="9"/>
@@ -4389,20 +4609,20 @@
       <c r="I93" s="9"/>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
-      <c r="L93" s="22"/>
-      <c r="M93" s="22"/>
-      <c r="N93" s="22"/>
-      <c r="O93" s="22"/>
-      <c r="P93" s="22"/>
-      <c r="Q93" s="22"/>
-      <c r="R93" s="22"/>
-      <c r="S93" s="23"/>
+      <c r="L93" s="9"/>
+      <c r="M93" s="19"/>
+      <c r="N93" s="19"/>
+      <c r="O93" s="19"/>
+      <c r="P93" s="19"/>
+      <c r="Q93" s="19"/>
+      <c r="R93" s="19"/>
+      <c r="S93" s="20"/>
     </row>
     <row r="94" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
-      <c r="D94" s="9"/>
+      <c r="D94" s="8"/>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
@@ -4410,20 +4630,20 @@
       <c r="I94" s="9"/>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
-      <c r="L94" s="22"/>
-      <c r="M94" s="22"/>
-      <c r="N94" s="22"/>
-      <c r="O94" s="22"/>
-      <c r="P94" s="22"/>
-      <c r="Q94" s="22"/>
-      <c r="R94" s="22"/>
-      <c r="S94" s="23"/>
+      <c r="L94" s="9"/>
+      <c r="M94" s="19"/>
+      <c r="N94" s="19"/>
+      <c r="O94" s="19"/>
+      <c r="P94" s="19"/>
+      <c r="Q94" s="19"/>
+      <c r="R94" s="19"/>
+      <c r="S94" s="20"/>
     </row>
     <row r="95" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
-      <c r="D95" s="9"/>
+      <c r="D95" s="8"/>
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
       <c r="G95" s="9"/>
@@ -4431,20 +4651,20 @@
       <c r="I95" s="9"/>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
-      <c r="L95" s="22"/>
-      <c r="M95" s="22"/>
-      <c r="N95" s="22"/>
-      <c r="O95" s="22"/>
-      <c r="P95" s="22"/>
-      <c r="Q95" s="22"/>
-      <c r="R95" s="22"/>
-      <c r="S95" s="23"/>
+      <c r="L95" s="9"/>
+      <c r="M95" s="19"/>
+      <c r="N95" s="19"/>
+      <c r="O95" s="19"/>
+      <c r="P95" s="19"/>
+      <c r="Q95" s="19"/>
+      <c r="R95" s="19"/>
+      <c r="S95" s="20"/>
     </row>
     <row r="96" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="9"/>
+      <c r="D96" s="8"/>
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
@@ -4452,20 +4672,20 @@
       <c r="I96" s="9"/>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
-      <c r="L96" s="22"/>
-      <c r="M96" s="22"/>
-      <c r="N96" s="22"/>
-      <c r="O96" s="22"/>
-      <c r="P96" s="22"/>
-      <c r="Q96" s="22"/>
-      <c r="R96" s="22"/>
-      <c r="S96" s="23"/>
+      <c r="L96" s="9"/>
+      <c r="M96" s="19"/>
+      <c r="N96" s="19"/>
+      <c r="O96" s="19"/>
+      <c r="P96" s="19"/>
+      <c r="Q96" s="19"/>
+      <c r="R96" s="19"/>
+      <c r="S96" s="20"/>
     </row>
     <row r="97" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="9"/>
+      <c r="D97" s="8"/>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
       <c r="G97" s="9"/>
@@ -4473,20 +4693,20 @@
       <c r="I97" s="9"/>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
-      <c r="L97" s="22"/>
-      <c r="M97" s="22"/>
-      <c r="N97" s="22"/>
-      <c r="O97" s="22"/>
-      <c r="P97" s="22"/>
-      <c r="Q97" s="22"/>
-      <c r="R97" s="22"/>
-      <c r="S97" s="23"/>
+      <c r="L97" s="9"/>
+      <c r="M97" s="19"/>
+      <c r="N97" s="19"/>
+      <c r="O97" s="19"/>
+      <c r="P97" s="19"/>
+      <c r="Q97" s="19"/>
+      <c r="R97" s="19"/>
+      <c r="S97" s="20"/>
     </row>
     <row r="98" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="9"/>
+      <c r="D98" s="8"/>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
@@ -4494,20 +4714,20 @@
       <c r="I98" s="9"/>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
-      <c r="L98" s="22"/>
-      <c r="M98" s="22"/>
-      <c r="N98" s="22"/>
-      <c r="O98" s="22"/>
-      <c r="P98" s="22"/>
-      <c r="Q98" s="22"/>
-      <c r="R98" s="22"/>
-      <c r="S98" s="23"/>
+      <c r="L98" s="9"/>
+      <c r="M98" s="19"/>
+      <c r="N98" s="19"/>
+      <c r="O98" s="19"/>
+      <c r="P98" s="19"/>
+      <c r="Q98" s="19"/>
+      <c r="R98" s="19"/>
+      <c r="S98" s="20"/>
     </row>
     <row r="99" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
-      <c r="D99" s="9"/>
+      <c r="D99" s="8"/>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
       <c r="G99" s="9"/>
@@ -4515,20 +4735,20 @@
       <c r="I99" s="9"/>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
-      <c r="L99" s="22"/>
-      <c r="M99" s="22"/>
-      <c r="N99" s="22"/>
-      <c r="O99" s="22"/>
-      <c r="P99" s="22"/>
-      <c r="Q99" s="22"/>
-      <c r="R99" s="22"/>
-      <c r="S99" s="23"/>
+      <c r="L99" s="9"/>
+      <c r="M99" s="19"/>
+      <c r="N99" s="19"/>
+      <c r="O99" s="19"/>
+      <c r="P99" s="19"/>
+      <c r="Q99" s="19"/>
+      <c r="R99" s="19"/>
+      <c r="S99" s="20"/>
     </row>
     <row r="100" spans="1:19" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
-      <c r="D100" s="9"/>
+      <c r="D100" s="8"/>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
       <c r="G100" s="9"/>
@@ -4536,18 +4756,18 @@
       <c r="I100" s="9"/>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
-      <c r="L100" s="22"/>
-      <c r="M100" s="22"/>
-      <c r="N100" s="22"/>
-      <c r="O100" s="22"/>
-      <c r="P100" s="22"/>
-      <c r="Q100" s="22"/>
-      <c r="R100" s="22"/>
-      <c r="S100" s="23"/>
+      <c r="L100" s="9"/>
+      <c r="M100" s="19"/>
+      <c r="N100" s="19"/>
+      <c r="O100" s="19"/>
+      <c r="P100" s="19"/>
+      <c r="Q100" s="19"/>
+      <c r="R100" s="19"/>
+      <c r="S100" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M1" r:id="rId1" xr:uid="{9B80FE5D-6B4B-4452-8753-71F3BE20CB96}"/>
+    <hyperlink ref="N1" r:id="rId1" xr:uid="{9B80FE5D-6B4B-4452-8753-71F3BE20CB96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>